<commit_message>
Lab 3 codes are updated...
</commit_message>
<xml_diff>
--- a/IE 211 Lab/src/Lab2/RunTimes.xlsx
+++ b/IE 211 Lab/src/Lab2/RunTimes.xlsx
@@ -229,7 +229,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
@@ -299,13 +299,13 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1016</c:v>
+                  <c:v>1147</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45680</c:v>
+                  <c:v>49029</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1370,7 +1370,7 @@
   <dimension ref="B1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1419,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
@@ -1430,7 +1430,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>1016</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
@@ -1441,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>45680</v>
+        <v>49029</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
@@ -1449,7 +1449,7 @@
         <v>500</v>
       </c>
       <c r="C7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1"/>
     </row>

</xml_diff>